<commit_message>
changed unknown dept to manual correction needed, add ability to manual name file with default settings as fallback
</commit_message>
<xml_diff>
--- a/Processed_Report.xlsx
+++ b/Processed_Report.xlsx
@@ -528,12 +528,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -602,12 +602,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -676,12 +676,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -750,12 +750,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -824,12 +824,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -898,12 +898,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -972,12 +972,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -1046,12 +1046,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -1120,12 +1120,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1194,12 +1194,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -1268,12 +1268,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1342,12 +1342,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -1416,12 +1416,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -1490,12 +1490,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1564,12 +1564,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -1638,12 +1638,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -1712,12 +1712,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -1786,12 +1786,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1860,12 +1860,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1934,12 +1934,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -2008,12 +2008,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -2082,12 +2082,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -2156,12 +2156,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -2230,12 +2230,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -2304,12 +2304,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -2378,12 +2378,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -2452,12 +2452,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -2526,12 +2526,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -2600,12 +2600,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -2674,12 +2674,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -2748,12 +2748,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -2822,12 +2822,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -2896,12 +2896,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -2970,12 +2970,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -3044,12 +3044,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -3118,12 +3118,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -3192,12 +3192,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -3266,12 +3266,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -3340,12 +3340,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -3414,12 +3414,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -3488,12 +3488,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -3562,12 +3562,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -3636,12 +3636,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -3710,12 +3710,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -3784,12 +3784,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -3858,12 +3858,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>10/01/2024</t>
+          <t>11/01/2024</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>11/01/2025</t>
+          <t>12/01/2025</t>
         </is>
       </c>
       <c r="C47" t="n">

</xml_diff>